<commit_message>
updated patch logistics, patient log updated by mohamad
</commit_message>
<xml_diff>
--- a/device-logistics.xlsx
+++ b/device-logistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahbook/Box Sync/projects/biobank/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asshah4\Box Sync\projects\biobank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B624E75-A267-0744-BB61-D72A89299AC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C922496-37A2-4459-A2F7-B7092E448109}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device-logistics" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="41">
   <si>
     <t>Device</t>
   </si>
@@ -124,13 +124,40 @@
   </si>
   <si>
     <t>DEV2</t>
+  </si>
+  <si>
+    <t>C700138</t>
+  </si>
+  <si>
+    <t>C700149</t>
+  </si>
+  <si>
+    <t>C700157</t>
+  </si>
+  <si>
+    <t>C700146</t>
+  </si>
+  <si>
+    <t>C700148</t>
+  </si>
+  <si>
+    <t>C700204</t>
+  </si>
+  <si>
+    <t>C700205</t>
+  </si>
+  <si>
+    <t>C700126</t>
+  </si>
+  <si>
+    <t>C700127</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -972,22 +999,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.125" customWidth="1"/>
-    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.375" customWidth="1"/>
-    <col min="4" max="4" width="17.625" customWidth="1"/>
+    <col min="1" max="1" width="23.08203125" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.58203125" customWidth="1"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1004,7 +1031,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="21">
+    <row r="2" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1019,7 +1046,7 @@
       </c>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:5" ht="21">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1036,7 +1063,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="21">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1047,11 +1074,11 @@
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" ht="21">
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1068,7 +1095,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="21">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1081,7 +1108,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" ht="21">
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1096,7 +1123,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="21">
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -1111,7 +1138,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="21">
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -1126,7 +1153,7 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" ht="21">
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1141,7 +1168,7 @@
       </c>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" ht="21">
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1158,7 +1185,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="21">
+    <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -1173,7 +1200,7 @@
       </c>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" ht="21">
+    <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
@@ -1184,11 +1211,11 @@
         <v>6</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="21">
+    <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -1199,11 +1226,11 @@
         <v>6</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" ht="21">
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -1218,7 +1245,7 @@
       </c>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" ht="21">
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1233,7 +1260,7 @@
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" ht="21">
+    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
@@ -1248,7 +1275,7 @@
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" ht="21">
+    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1259,11 +1286,11 @@
         <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" ht="21">
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1274,7 +1301,259 @@
         <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A30" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.5">
+      <c r="A32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.5">
+      <c r="A33" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.5">
+      <c r="A34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.5">
+      <c r="A35" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.5">
+      <c r="A36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.5">
+      <c r="A37" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added team project, updated location of manuscript, updated patch logistics for most recent lost device
</commit_message>
<xml_diff>
--- a/device-logistics.xlsx
+++ b/device-logistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asshah4\Box Sync\projects\biobank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C922496-37A2-4459-A2F7-B7092E448109}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C0F99D-95E0-4885-B5A0-C65E4639DCC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device-logistics" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="46">
   <si>
     <t>Device</t>
   </si>
@@ -151,6 +151,21 @@
   </si>
   <si>
     <t>C700127</t>
+  </si>
+  <si>
+    <t>MRN: 1303033</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>ANDROID7</t>
+  </si>
+  <si>
+    <t>Pratik</t>
+  </si>
+  <si>
+    <t>Unable to log-in</t>
   </si>
 </sst>
 </file>
@@ -999,10 +1014,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1155,57 +1170,59 @@
     </row>
     <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>24</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>6</v>
@@ -1220,7 +1237,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
@@ -1232,13 +1249,13 @@
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>8</v>
@@ -1250,10 +1267,10 @@
         <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>8</v>
@@ -1265,10 +1282,10 @@
         <v>28</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>8</v>
@@ -1280,10 +1297,10 @@
         <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
@@ -1295,7 +1312,7 @@
         <v>28</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>6</v>
@@ -1303,19 +1320,23 @@
       <c r="D19" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.5">
@@ -1323,7 +1344,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
@@ -1337,7 +1358,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>6</v>
@@ -1351,7 +1372,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>6</v>
@@ -1365,7 +1386,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
@@ -1379,7 +1400,7 @@
         <v>20</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
@@ -1393,7 +1414,7 @@
         <v>20</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>6</v>
@@ -1407,7 +1428,7 @@
         <v>20</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
@@ -1421,7 +1442,7 @@
         <v>20</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>6</v>
@@ -1432,10 +1453,10 @@
     </row>
     <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>6</v>
@@ -1449,7 +1470,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>6</v>
@@ -1463,7 +1484,7 @@
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>6</v>
@@ -1477,7 +1498,7 @@
         <v>28</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>6</v>
@@ -1491,7 +1512,7 @@
         <v>28</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>6</v>
@@ -1505,7 +1526,7 @@
         <v>28</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>6</v>
@@ -1519,7 +1540,7 @@
         <v>28</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>6</v>
@@ -1533,7 +1554,7 @@
         <v>28</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>6</v>
@@ -1547,12 +1568,26 @@
         <v>28</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.5">
+      <c r="A38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" s="1" t="s">
+      <c r="C38" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated adding new columns to project, categorized the MOCA score
</commit_message>
<xml_diff>
--- a/device-logistics.xlsx
+++ b/device-logistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asshah4\Box Sync\projects\biobank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C0F99D-95E0-4885-B5A0-C65E4639DCC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE00E8AB-BE65-461B-9E6A-A6496119E281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="device-logistics" sheetId="1" r:id="rId1"/>
@@ -60,9 +60,6 @@
     <t>MOB2</t>
   </si>
   <si>
-    <t>Blue tooth issues</t>
-  </si>
-  <si>
     <t>MOB3</t>
   </si>
   <si>
@@ -166,6 +163,9 @@
   </si>
   <si>
     <t>Unable to log-in</t>
+  </si>
+  <si>
+    <t>Bluetooth issues in past, trying to use again 1/29/20</t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1017,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1075,7 +1075,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.5">
@@ -1086,7 +1086,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
@@ -1101,13 +1101,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.5">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>8</v>
@@ -1129,13 +1129,13 @@
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.5">
@@ -1144,13 +1144,13 @@
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.5">
@@ -1161,7 +1161,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>8</v>
@@ -1173,24 +1173,24 @@
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>6</v>
@@ -1202,27 +1202,27 @@
     </row>
     <row r="12" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>6</v>
@@ -1234,10 +1234,10 @@
     </row>
     <row r="14" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
@@ -1249,10 +1249,10 @@
     </row>
     <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>6</v>
@@ -1264,13 +1264,13 @@
     </row>
     <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>8</v>
@@ -1279,13 +1279,13 @@
     </row>
     <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>8</v>
@@ -1294,13 +1294,13 @@
     </row>
     <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
@@ -1309,10 +1309,10 @@
     </row>
     <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>6</v>
@@ -1324,27 +1324,27 @@
     </row>
     <row r="20" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
@@ -1355,10 +1355,10 @@
     </row>
     <row r="22" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>6</v>
@@ -1369,10 +1369,10 @@
     </row>
     <row r="23" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A23" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>6</v>
@@ -1383,10 +1383,10 @@
     </row>
     <row r="24" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A24" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>6</v>
@@ -1397,10 +1397,10 @@
     </row>
     <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A25" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>6</v>
@@ -1411,10 +1411,10 @@
     </row>
     <row r="26" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A26" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>6</v>
@@ -1425,10 +1425,10 @@
     </row>
     <row r="27" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A27" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>6</v>
@@ -1439,10 +1439,10 @@
     </row>
     <row r="28" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A28" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>6</v>
@@ -1453,10 +1453,10 @@
     </row>
     <row r="29" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A29" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>6</v>
@@ -1467,10 +1467,10 @@
     </row>
     <row r="30" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A30" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>6</v>
@@ -1481,10 +1481,10 @@
     </row>
     <row r="31" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A31" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>6</v>
@@ -1495,10 +1495,10 @@
     </row>
     <row r="32" spans="1:5" ht="21" x14ac:dyDescent="0.5">
       <c r="A32" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>6</v>
@@ -1509,10 +1509,10 @@
     </row>
     <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.5">
       <c r="A33" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>6</v>
@@ -1523,10 +1523,10 @@
     </row>
     <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.5">
       <c r="A34" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>6</v>
@@ -1537,10 +1537,10 @@
     </row>
     <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.5">
       <c r="A35" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>6</v>
@@ -1551,10 +1551,10 @@
     </row>
     <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.5">
       <c r="A36" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>6</v>
@@ -1565,10 +1565,10 @@
     </row>
     <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.5">
       <c r="A37" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>6</v>
@@ -1579,10 +1579,10 @@
     </row>
     <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.5">
       <c r="A38" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>6</v>

</xml_diff>